<commit_message>
Added random color function to Word/HashtagCloud for a more fitting color scheme
</commit_message>
<xml_diff>
--- a/TwitterSentimentAnalyser/TSentimentAnalyser/static/raw_tweets.xlsx
+++ b/TwitterSentimentAnalyser/TSentimentAnalyser/static/raw_tweets.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,48 +506,52 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>@CBSNews #tRUmp will fuck with the EC. Just watch him. Miller says they have their own hand picked collection of el… https://t.co/X7WRevFSEu</t>
+          <t>RT @G0rille: 🔴 #BidenHarris2020 ce vieux croulant aurait fait 80 millions de votes. Sa femme vient le guider, il est perdu. On nous prend p…</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1.338492216336126e+18</v>
+        <v>1.33876185976848e+18</v>
       </c>
       <c r="D2" t="n">
         <v>140</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>44179.60633101852</v>
+        <v>44180.35040509259</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>fr</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>1.134776212344254e+18</v>
+        <v>3391244362</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>aahpat01</t>
+          <t>PorcinetteLouis</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>220</v>
-      </c>
-      <c r="J2" t="inlineStr"/>
+        <v>1257</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Zambie</t>
+        </is>
+      </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t xml:space="preserve">@CBSNews #tRUmp will fuck with the EC. Just watch him. Miller says they have their own hand picked collection of el… https://t.co/X7WRevFSEu </t>
+          <t xml:space="preserve">RT @ G0rille: 🔴 # BidenHarris2020 this crumbling old man would have had 80 million votes. His wife comes to guide him, he is lost. We are taken p ... </t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> #tRUmp will fuck with the EC. Just watch him. Miller says they have their own hand picked collection of el… </t>
+          <t xml:space="preserve"> 🔴 #BidenHarris2020 ce vieux croulant aurait fait 80 millions de votes. Sa femme vient le guider, il est perdu. On nous prend p…</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> #tRUmp will fuck with the EC. Just watch him. Miller says they have their own hand picked collection of el…  </t>
+          <t xml:space="preserve">RT  G0rille: 🔴 # BidenHarris2020 this crumbling old man would have had 80 million votes. His wife comes to guide him, he is lost. We are taken p ... </t>
         </is>
       </c>
     </row>
@@ -557,18 +561,20 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Russian Hackers Broke Into Federal Agencies, U.S. Officials Suspect
-#NationalSecurity #hacker #PENTAGON #trump… https://t.co/AesxnWHb9Z</t>
+          <t>This is Donald Trump's "bone spur" x-ray finally released...😅
+#TrumpIsALaughingStock 
+#Trump 
+#TrumpMeltdown https://t.co/dfNybDGV4X</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1.338492212959719e+18</v>
+        <v>1.3387618431925e+18</v>
       </c>
       <c r="D3" t="n">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>44179.60631944444</v>
+        <v>44180.3503587963</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -576,31 +582,33 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>1.275777664180269e+18</v>
+        <v>1.313864684429337e+18</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>ScottyJo1989</t>
+          <t>Leonard59554150</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>3727</v>
+        <v>278</v>
       </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Russian Hackers Broke Into Federal Agencies, U.S. Officials Suspect#NationalSecurity #hacker #PENTAGON #trump… https://t.co/AesxnWHb9Z </t>
+          <t xml:space="preserve">This is Donald Trump's "bone spur" x-ray finally released...😅#TrumpIsALaughingStock #Trump #TrumpMeltdown https://t.co/dfNybDGV4X </t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Russian Hackers Broke Into Federal Agencies, U.S. Officials Suspect
-#NationalSecurity #hacker #PENTAGON #trump… </t>
+          <t xml:space="preserve">This is Donald Trump's "bone spur" x-ray finally released...😅
+#TrumpIsALaughingStock 
+#Trump 
+#TrumpMeltdown </t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Russian Hackers Broke Into Federal Agencies, U.S. Officials Suspect#NationalSecurity #hacker #PENTAGON #trump…  </t>
+          <t xml:space="preserve">This is Donald Trump's "bone spur" x-ray finally released...😅#TrumpIsALaughingStock #Trump #TrumpMeltdown  </t>
         </is>
       </c>
     </row>
@@ -610,52 +618,52 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>@Tia6sc @Truthseeker126 @POTUS @VP @FLOTUS @SecondLady #China just sent Biden his speech and the plans for his admi… https://t.co/NVkgfD8eQe</t>
+          <t>RT @URDUVOA: ریاست ڈیلاویئر کے شہر ولمنگٹن سے اپنے خطاب میں بائیڈن نے کہا کہ ملک میں حکمرانی کے اُصولوں کو آزمائش میں ڈالا گیا، دھمکیاں دی…</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.338492195700158e+18</v>
+        <v>1.338761838352355e+18</v>
       </c>
       <c r="D4" t="n">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>44179.60627314815</v>
+        <v>44180.35033564815</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>ur</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>1117593438</v>
+        <v>1.259103255063409e+18</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>SSDavidT</t>
+          <t>logazihall</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>5452</v>
+        <v>362</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t xml:space="preserve">@Tia6sc @Truthseeker126 @POTUS @VP @FLOTUS @SecondLady #China just sent Biden his speech and the plans for his admi… https://t.co/NVkgfD8eQe </t>
+          <t xml:space="preserve">RT @URDUVOA: In his address from Wilmington, Delaware, Biden said that the principles of governance in the country have been tested and threatened. </t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t xml:space="preserve">      #China just sent Biden his speech and the plans for his admi… </t>
+          <t xml:space="preserve"> ریاست ڈیلاویئر کے شہر ولمنگٹن سے اپنے خطاب میں بائیڈن نے کہا کہ ملک میں حکمرانی کے اُصولوں کو آزمائش میں ڈالا گیا، دھمکیاں دی…</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t xml:space="preserve">      #China just sent Biden his speech and the plans for his admi…  </t>
+          <t xml:space="preserve"> In his address from Wilmington, Delaware, Biden said that the principles of governance in the country have been tested and threatened. </t>
         </is>
       </c>
     </row>
@@ -665,52 +673,52 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>RT @RTenfrancais: Des élus américains demandent à #Trump d'amnistier #Snowden
-#EtatsUnis🇺🇸 
-➡️https://t.co/3nEYVi2hxp https://t.co/MAvAdr…</t>
+          <t>#AunqueNoGusteATodos Joe Biden es el ganador de las elecciones presidenciales en #EEUU. El primero que debe asumirl… https://t.co/zqe5FWhzpv</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1.338492174573433e+18</v>
+        <v>1.338761810997092e+18</v>
       </c>
       <c r="D5" t="n">
         <v>140</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>44179.60621527778</v>
+        <v>44180.35026620371</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>fr</t>
+          <t>es</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>1.261184438244966e+18</v>
+        <v>1058557477</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>fabienne_mimi</t>
+          <t>ahlamry</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>252</v>
-      </c>
-      <c r="J5" t="inlineStr"/>
+        <v>241</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Mota Del Cuervo - Madrid</t>
+        </is>
+      </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @RTenfrancais: American elected officials ask #Trump for amnesty # Snowden # United States🇺🇸 ➡️https: //t.co/3nEYVi2hxp https://t.co/MAvAdr… </t>
+          <t xml:space="preserve">#AunqueNotLikeAll Joe Biden is the winner of the presidential elections in #USA. The first thing you should assume… https://t.co/zqe5FWhzpv </t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Des élus américains demandent à #Trump d'amnistier #Snowden
-#EtatsUnis🇺🇸 
-➡️ …</t>
+          <t xml:space="preserve">#AunqueNoGusteATodos Joe Biden es el ganador de las elecciones presidenciales en #EEUU. El primero que debe asumirl… </t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> American elected officials ask #Trump for amnesty # Snowden # United States🇺🇸 ➡️https: //t.co/3nEYVi2hxp … </t>
+          <t xml:space="preserve">#AunqueNotLikeAll Joe Biden is the winner of the presidential elections in #USA. The first thing you should assume…  </t>
         </is>
       </c>
     </row>
@@ -720,323 +728,48 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>I’d take a #Trump-approved vaccine way before a #Trudeau- approved one. 
-We know Trudeau sources the injection mat… https://t.co/rsFxtWYFwK</t>
+          <t>RT @MarocVortex: 20ans de règne Al hamdoulilah ! Qu'Allah préserve Sa Majesté le Roi #MohammedVI et mes frères et soeurs #Marocain(e)s #Mon…</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1.338492159020982e+18</v>
+        <v>1.338761791879385e+18</v>
       </c>
       <c r="D6" t="n">
         <v>140</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>44179.60616898148</v>
+        <v>44180.35020833334</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>fr</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>1.255952793673896e+18</v>
+        <v>1.212375946696647e+18</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>VeinVigri</t>
+          <t>timbalandmago</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>92</v>
+        <v>762</v>
       </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr">
         <is>
-          <t xml:space="preserve">I’d take a #Trump-approved vaccine way before a #Trudeau- approved one. We know Trudeau sources the injection mat… https://t.co/rsFxtWYFwK </t>
+          <t xml:space="preserve">RT @MarocVortex: 20 years of reign Al hamdoulilah! May Allah preserve His Majesty the King #MohammedVI and my brothers and sisters #Moroccans # My… </t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t xml:space="preserve">I’d take a #Trump-approved vaccine way before a #Trudeau- approved one. 
-We know Trudeau sources the injection mat… </t>
+          <t xml:space="preserve"> 20ans de règne Al hamdoulilah ! Qu'Allah préserve Sa Majesté le Roi #MohammedVI et mes frères et soeurs #Marocain(e)s #Mon…</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t xml:space="preserve">I’d take a #Trump-approved vaccine way before a #Trudeau- approved one. We know Trudeau sources the injection mat…  </t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>RT @KrauseForIowa: #Mueller identified quite a few moles who'd gathered around #Trump very early on. Is it likely, given size of the espion…</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>1.338492156550414e+18</v>
-      </c>
-      <c r="D7" t="n">
-        <v>140</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>44179.6061574074</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
-        <v>2296781690</v>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>keffberrystrien</t>
-        </is>
-      </c>
-      <c r="I7" t="n">
-        <v>297</v>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>United States</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">RT @KrauseForIowa: #Mueller identified quite a few moles who'd gathered around #Trump very early on. Is it likely, given size of the espion… </t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> #Mueller identified quite a few moles who'd gathered around #Trump very early on. Is it likely, given size of the espion…</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> #Mueller identified quite a few moles who'd gathered around #Trump very early on. Is it likely, given size of the espion… </t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>#Trump #USA : "Premier vaccin administré. Félicitations aux USA! Félicitations au MONDE!" https://t.co/SHK8lLjjsK</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>1.33849215418479e+18</v>
-      </c>
-      <c r="D8" t="n">
-        <v>113</v>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>44179.6061574074</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>fr</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
-        <v>1.116278323410239e+18</v>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>SaveMeUp1</t>
-        </is>
-      </c>
-      <c r="I8" t="n">
-        <v>129</v>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>Singapore</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">#Trump #USA: "First vaccine administered. Congratulations to the USA! Congratulations to the WORLD!" https://t.co/SHK8lLjjsK </t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">#Trump #USA : "Premier vaccin administré. Félicitations aux USA! Félicitations au MONDE!" </t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">#Trump #USA: "First vaccine administered. Congratulations to the USA! Congratulations to the WORLD!"  </t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>RT @RTenfrancais: Des élus américains demandent à #Trump d'amnistier #Snowden
-#EtatsUnis🇺🇸 
-➡️https://t.co/3nEYVi2hxp https://t.co/MAvAdr…</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>1.3384921415726e+18</v>
-      </c>
-      <c r="D9" t="n">
-        <v>140</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>44179.60612268518</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>fr</t>
-        </is>
-      </c>
-      <c r="G9" t="n">
-        <v>1.307708458284786e+18</v>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Christi22917002</t>
-        </is>
-      </c>
-      <c r="I9" t="n">
-        <v>163</v>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>Caudry , NORD</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">RT @RTenfrancais: American elected officials ask #Trump for amnesty # Snowden # United States🇺🇸 ➡️https: //t.co/3nEYVi2hxp https://t.co/MAvAdr… </t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Des élus américains demandent à #Trump d'amnistier #Snowden
-#EtatsUnis🇺🇸 
-➡️ …</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> American elected officials ask #Trump for amnesty # Snowden # United States🇺🇸 ➡️https: //t.co/3nEYVi2hxp … </t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>E notizia di oggi anche attacco hacker multiplo (compreso a #Google dunque anche #YouTubeDOWN )
-Sempre e rigorosame… https://t.co/glOEBcrp5B</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>1.338492113282101e+18</v>
-      </c>
-      <c r="D10" t="n">
-        <v>140</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>44179.60604166667</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>it</t>
-        </is>
-      </c>
-      <c r="G10" t="n">
-        <v>4147420395</v>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>erospoeta1</t>
-        </is>
-      </c>
-      <c r="I10" t="n">
-        <v>56</v>
-      </c>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">And today's news is also a multiple hacker attack (including #Google and therefore also #YouTubeDOWN) Always and rigorously… https://t.co/glOEBcrp5B </t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">E notizia di oggi anche attacco hacker multiplo (compreso a #Google dunque anche #YouTubeDOWN )
-Sempre e rigorosame… </t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">And today's news is also a multiple hacker attack (including #Google and therefore also #YouTubeDOWN) Always and rigorously…  </t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>You can earn $1,000 to play the new PS5 — and get to keep the console ***RESTOCKS*** SEE MORE HERE ==&amp;gt;… https://t.co/yl1UjBqAFd</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>1.338492106986426e+18</v>
-      </c>
-      <c r="D11" t="n">
-        <v>130</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>44179.60601851852</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="G11" t="n">
-        <v>306127388</v>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>bitcoinconnect</t>
-        </is>
-      </c>
-      <c r="I11" t="n">
-        <v>1230</v>
-      </c>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">You can earn $1,000 to play the new PS5 — and get to keep the console ***RESTOCKS*** SEE MORE HERE ==&amp;gt;… https://t.co/yl1UjBqAFd </t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">You can earn $1,000 to play the new PS5 — and get to keep the console ***RESTOCKS*** SEE MORE HERE ==&amp;gt;… </t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">You can earn $1,000 to play the new PS5 — and get to keep the console ***RESTOCKS*** SEE MORE HERE ==&amp;gt;…  </t>
+          <t xml:space="preserve"> 20 years of reign Al hamdoulilah! May Allah preserve His Majesty the King #MohammedVI and my brothers and sisters #Moroccans # My… </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added some text to FAQ and recolored home.html Title Text
</commit_message>
<xml_diff>
--- a/TwitterSentimentAnalyser/TSentimentAnalyser/static/raw_tweets.xlsx
+++ b/TwitterSentimentAnalyser/TSentimentAnalyser/static/raw_tweets.xlsx
@@ -506,52 +506,60 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>RT @santangelo_s: Grazie a tutti i lettori che - con la loro attenzione - stanno decretando il successo di #Geopandemia @CastelvecchiEd #CO…</t>
+          <t>#Trump announced that he would fire #WilliamBarr.
+.
+.
+He reminds me of children ...😑
+#TrumpIsACriminal… https://t.co/1B51buQrc6</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1.338817358610174e+18</v>
+        <v>1.338856399380623e+18</v>
       </c>
       <c r="D2" t="n">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>44180.50354166667</v>
+        <v>44180.61128472222</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>it</t>
+          <t>en</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>1377704858</v>
+        <v>1.273713204242395e+18</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>startzai</t>
+          <t>Ashleysullivan_</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>3936</v>
+        <v>596</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>italy</t>
+          <t>Chicago</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @santangelo_s: Thanks to all the readers who - with their attention - are decreeing the success of #Geopandemia @CastelvecchiEd # CO ... </t>
+          <t xml:space="preserve">#Trump announced that he would fire #WilliamBarr...He reminds me of children ...😑#TrumpIsACriminal… https://t.co/1B51buQrc6 </t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Grazie a tutti i lettori che - con la loro attenzione - stanno decretando il successo di #Geopandemia  #CO…</t>
+          <t xml:space="preserve">#Trump announced that he would fire #WilliamBarr.
+.
+.
+He reminds me of children ...😑
+#TrumpIsACriminal… </t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Thanks to all the readers who - with their attention - are decreeing the success of #Geopandemia  # CO ... </t>
+          <t xml:space="preserve">#Trump announced that he would fire #WilliamBarr...He reminds me of children ...😑#TrumpIsACriminal…  </t>
         </is>
       </c>
     </row>
@@ -561,60 +569,48 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>RT @Trump_Fact_News: 🚨Breaking
-✅GÉORGIE
-✅ PENNSYLVANIE
-✅ NEVADA
-Les républicains de ces États ont voté pour le président #Trump. Ce sont m…</t>
+          <t>RT @ManDessins: #COVID19 #USA #Trump #Dessin @Midilibre https://t.co/hv8DQwBzIc</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1.338817320119116e+18</v>
+        <v>1.3388563888234e+18</v>
       </c>
       <c r="D3" t="n">
-        <v>140</v>
+        <v>79</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>44180.5034375</v>
+        <v>44180.61125</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>fr</t>
+          <t>und</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>1241669749</v>
+        <v>604704562</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>JstLangevin</t>
+          <t>bonsoirmichel</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>16149</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>france</t>
-        </is>
-      </c>
+        <v>13262</v>
+      </c>
+      <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @Trump_Fact_News: 🚨Breaking✅GEORGIA✅ PENNSYLVANIA✅ NEVADAL Republicans in those states voted for President #Trump. These are m ... </t>
+          <t xml:space="preserve">RT @ManDessins: # COVID19 #USA #Trump #Dessin @Midilibre https://t.co/hv8DQwBzIc </t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 🚨Breaking
-✅GÉORGIE
-✅ PENNSYLVANIE
-✅ NEVADA
-Les républicains de ces États ont voté pour le président #Trump. Ce sont m…</t>
+          <t xml:space="preserve"> #COVID19 #USA #Trump #Dessin  </t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 🚨Breaking✅GEORGIA✅ PENNSYLVANIA✅ NEVADAL Republicans in those states voted for President #Trump. These are m ... </t>
+          <t xml:space="preserve"> # COVID19 #USA #Trump #Dessin   </t>
         </is>
       </c>
     </row>
@@ -624,48 +620,56 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>RT @Fr_Conservateur: #Zemmour : « Financés par la Grande bourgeoisie, les stars d'Hollywood, par les groupes de #Soros, qui financent déjà…</t>
+          <t>#Trump 
+this is the end
+Jim Morrison</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.338817317711573e+18</v>
+        <v>1.338856381877604e+18</v>
       </c>
       <c r="D4" t="n">
-        <v>139</v>
+        <v>37</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>44180.5034375</v>
+        <v>44180.61122685186</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>fr</t>
+          <t>en</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>587227597</v>
+        <v>16604304</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>BernRAH</t>
+          <t>muehlenwind</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>1634</v>
-      </c>
-      <c r="J4" t="inlineStr"/>
+        <v>2340</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Sandstrand, Deutschland</t>
+        </is>
+      </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @Fr_Conservateur: #Zemmour: “Financed by the upper middle class, the Hollywood stars, by the #Soros groups, which are already financing… </t>
+          <t xml:space="preserve">#Trump this is the endJim Morrison </t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> #Zemmour : « Financés par la Grande bourgeoisie, les stars d'Hollywood, par les groupes de #Soros, qui financent déjà…</t>
+          <t>#Trump 
+this is the end
+Jim Morrison</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> #Zemmour: “Financed by the upper middle class, the Hollywood stars, by the #Soros groups, which are already financing… </t>
+          <t xml:space="preserve">#Trump this is the endJim Morrison </t>
         </is>
       </c>
     </row>
@@ -675,48 +679,52 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>RT @Danilo_Sant65: #Trump liquida #Barr :”Ho appena avuto un incontro molto carino con il procuratore Bill Barr. Il nostro rapporto è stato…</t>
+          <t>@NotHoodlum Why is everyone so shocked? It’s the one promise #Trump kept - the entitled get more entitlement.… https://t.co/I95RVALzIQ</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1.338817317581545e+18</v>
+        <v>1.338856364635009e+18</v>
       </c>
       <c r="D5" t="n">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>44180.5034375</v>
+        <v>44180.61118055556</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>it</t>
+          <t>en</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>2893414655</v>
+        <v>757529364</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>guerrini193</t>
+          <t>MillieMinet</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>93</v>
-      </c>
-      <c r="J5" t="inlineStr"/>
+        <v>615</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>NPT</t>
+        </is>
+      </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @ Danilo_Sant65: #Trump liquidates #Barr: “I just had a very nice meeting with DA Bill Barr. Our relationship was ... </t>
+          <t xml:space="preserve">@NotHoodlum Why is everyone so shocked? It’s the one promise #Trump kept - the entitled get more entitlement.… https://t.co/I95RVALzIQ </t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> #Trump liquida #Barr :”Ho appena avuto un incontro molto carino con il procuratore Bill Barr. Il nostro rapporto è stato…</t>
+          <t xml:space="preserve"> Why is everyone so shocked? It’s the one promise #Trump kept - the entitled get more entitlement.… </t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT  Danilo_Sant65: #Trump liquidates #Barr: “I just had a very nice meeting with DA Bill Barr. Our relationship was ... </t>
+          <t xml:space="preserve"> Why is everyone so shocked? It’s the one promise #Trump kept - the entitled get more entitlement.…  </t>
         </is>
       </c>
     </row>
@@ -726,52 +734,52 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>@DavidJimenezTW coincido con David. Quiero ver a #Trump salir de la Casa Blanca pataleando, conducido en volandas p… https://t.co/IcPA96n86C</t>
+          <t>President Donald #Trump stands among Army cadets as he attends the annual Army-Navy collegiate football game in… https://t.co/P7nglPVrEb</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1.338817316969177e+18</v>
+        <v>1.338856361669616e+18</v>
       </c>
       <c r="D6" t="n">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>44180.5034375</v>
+        <v>44180.61118055556</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>es</t>
+          <t>en</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>2389078194</v>
+        <v>8.42343300115927e+17</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>sllopisortega</t>
+          <t>pow_photos</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1424</v>
+        <v>806</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Madrid, Comunidad de Madrid</t>
+          <t>Lebanon</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t xml:space="preserve">@DavidJimenezTW I agree with David. I want to see #Trump leave the White House kicking, driven in flying p… https://t.co/IcPA96n86C </t>
+          <t xml:space="preserve">President Donald #Trump stands among Army cadets as he attends the annual Army-Navy collegiate football game in… https://t.co/P7nglPVrEb </t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> coincido con David. Quiero ver a #Trump salir de la Casa Blanca pataleando, conducido en volandas p… </t>
+          <t xml:space="preserve">President Donald #Trump stands among Army cadets as he attends the annual Army-Navy collegiate football game in… </t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> I agree with David. I want to see #Trump leave the White House kicking, driven in flying p…  </t>
+          <t xml:space="preserve">President Donald #Trump stands among Army cadets as he attends the annual Army-Navy collegiate football game in…  </t>
         </is>
       </c>
     </row>
@@ -781,48 +789,54 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Couverture parfaite, le pire Président des Usa Qu’il est existé et il va enfin partir le décérébré dangereux populi… https://t.co/3im1lGUmqw</t>
+          <t>The electoral college has spoken. YOU LOST AGAIN. Perhaps #Trump is bad for America. 
+#ShutHimOut… https://t.co/1w7CuvK9Ri</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1.338817308622516e+18</v>
+        <v>1.338856349032178e+18</v>
       </c>
       <c r="D7" t="n">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>44180.50341435185</v>
+        <v>44180.61114583333</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>fr</t>
+          <t>en</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>1510467566</v>
+        <v>267129243</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>CnathDreamer</t>
+          <t>TarikuBogale</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>407</v>
-      </c>
-      <c r="J7" t="inlineStr"/>
+        <v>5466</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>New York</t>
+        </is>
+      </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Perfect cover, the worst President of the Usa He ever existed and he will finally leave the dangerous mindless populi ... https://t.co/3im1lGUmqw </t>
+          <t xml:space="preserve">The electoral college has spoken. YOU LOST AGAIN. Perhaps #Trump is bad for America. #ShutHimOut… https://t.co/1w7CuvK9Ri </t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Couverture parfaite, le pire Président des Usa Qu’il est existé et il va enfin partir le décérébré dangereux populi… </t>
+          <t xml:space="preserve">The electoral college has spoken. YOU LOST AGAIN. Perhaps #Trump is bad for America. 
+#ShutHimOut… </t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Perfect cover, the worst President of the Usa He ever existed and he will finally leave the dangerous mindless populi ...  </t>
+          <t xml:space="preserve">The electoral college has spoken. YOU LOST AGAIN. Perhaps #Trump is bad for America. #ShutHimOut…  </t>
         </is>
       </c>
     </row>
@@ -832,48 +846,54 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>En 2016 @libe expliquait que les grands électeurs pouvaient voter Clinton alors que trump avait gagné dans leur éta… https://t.co/tbuNWEtc8s</t>
+          <t>RT @AlexdGtze: @washingtonpost Truth hurts
+#BidenVaccine #Trump https://t.co/1e8oIOxc5y</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1.338817305950753e+18</v>
+        <v>1.338856347044033e+18</v>
       </c>
       <c r="D8" t="n">
-        <v>140</v>
+        <v>87</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>44180.50340277778</v>
+        <v>44180.61113425926</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>fr</t>
+          <t>en</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>1668375678</v>
+        <v>1.259356052635542e+18</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>fabien_lanfr</t>
+          <t>JoeKing84576078</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>404</v>
-      </c>
-      <c r="J8" t="inlineStr"/>
+        <v>511</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Texas, USA</t>
+        </is>
+      </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t xml:space="preserve">In 2016 @libe explained that big voters could vote for Clinton when Trump won in their state… https://t.co/tbuNWEtc8s </t>
+          <t xml:space="preserve">RT @AlexdGtze: @washingtonpost Truth hurts#BidenVaccine #Trump https://t.co/1e8oIOxc5y </t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t xml:space="preserve">En 2016  expliquait que les grands électeurs pouvaient voter Clinton alors que trump avait gagné dans leur éta… </t>
+          <t xml:space="preserve">  Truth hurts
+#BidenVaccine #Trump </t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t xml:space="preserve">In 2016  explained that big voters could vote for Clinton when Trump won in their state…  </t>
+          <t xml:space="preserve">  Truth hurts#BidenVaccine #Trump  </t>
         </is>
       </c>
     </row>
@@ -883,48 +903,48 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Por fiiiiin!! Adiós #Trump, good bye, arrivederci, adéu y deja de joder ya con tus pelotitas. Cansino, el jodío... https://t.co/GAp9eU1HjP</t>
+          <t>@mkraju Strongly disagree with vacs for #Trump and #Pence. They have been advocating for super-spreading since the… https://t.co/Jm35wvOwH1</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1.338817276842283e+18</v>
+        <v>1.338856345882096e+18</v>
       </c>
       <c r="D9" t="n">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>44180.50332175926</v>
+        <v>44180.61113425926</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>es</t>
+          <t>en</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>8.553723090032108e+17</v>
+        <v>1.229178950347149e+18</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>somnormals</t>
+          <t>LAShake2</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>1952</v>
+        <v>7</v>
       </c>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr">
         <is>
-          <t xml:space="preserve">By fiiiiin !! Goodbye #Trump, good bye, arrivederci, adéu and stop fucking with your balls. Cansino, the screwed up ... https://t.co/GAp9eU1HjP </t>
+          <t xml:space="preserve">@mkraju Strongly disagree with vacs for #Trump and #Pence. They have been advocating for super-spreading since the… https://t.co/Jm35wvOwH1 </t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Por fiiiiin!! Adiós #Trump, good bye, arrivederci, adéu y deja de joder ya con tus pelotitas. Cansino, el jodío... </t>
+          <t xml:space="preserve"> Strongly disagree with vacs for #Trump and #Pence. They have been advocating for super-spreading since the… </t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t xml:space="preserve">By fiiiiin !! Goodbye #Trump, good bye, arrivederci, adéu and stop fucking with your balls. Cansino, the screwed up ...  </t>
+          <t xml:space="preserve"> Strongly disagree with vacs for #Trump and #Pence. They have been advocating for super-spreading since the…  </t>
         </is>
       </c>
     </row>
@@ -934,17 +954,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>“We will presumably get more certainty in days ahead about whether #Russia did this #hack, as well as the many key… https://t.co/HerITn0kEr</t>
+          <t>@JoeBiden We all know you cheated. The sad thing is, YOU probably don’t know you cheated. The audacity to write thi… https://t.co/wXz7eT8rMF</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1.338817268847792e+18</v>
+        <v>1.338856318673809e+18</v>
       </c>
       <c r="D10" t="n">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>44180.50329861111</v>
+        <v>44180.61105324074</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -952,30 +972,34 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>1.190795199754252e+18</v>
+        <v>1.298013110691758e+18</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>freyjja5</t>
+          <t>JiruJoshua</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>8922</v>
-      </c>
-      <c r="J10" t="inlineStr"/>
+        <v>17</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Madison, WI</t>
+        </is>
+      </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t xml:space="preserve">“We will presumably get more certainty in days ahead about whether #Russia did this #hack, as well as the many key… https://t.co/HerITn0kEr </t>
+          <t xml:space="preserve">@JoeBiden We all know you cheated. The sad thing is, YOU probably don’t know you cheated. The audacity to write thi… https://t.co/wXz7eT8rMF </t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t xml:space="preserve">“We will presumably get more certainty in days ahead about whether #Russia did this #hack, as well as the many key… </t>
+          <t xml:space="preserve"> We all know you cheated. The sad thing is, YOU probably don’t know you cheated. The audacity to write thi… </t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t xml:space="preserve">“We will presumably get more certainty in days ahead about whether #Russia did this #hack, as well as the many key…  </t>
+          <t xml:space="preserve"> We all know you cheated. The sad thing is, YOU probably don’t know you cheated. The audacity to write thi…  </t>
         </is>
       </c>
     </row>
@@ -985,50 +1009,48 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>.@realDonaldTrump  : You, sir, are the reason God created the middle finger.
-#ByeHannity #JoeBiden #Trump… https://t.co/7FsHgeINrG</t>
+          <t>RT @JUANdeITALIA: El presidente MR #TRUMP sea como sea EL en su conducta imperfecta ...es un patriota además de persona creyente en DIOS, t…</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1.338817233657733e+18</v>
+        <v>1.338856311044321e+18</v>
       </c>
       <c r="D11" t="n">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>44180.50320601852</v>
+        <v>44180.61103009259</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>es</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>150982697</v>
+        <v>353243516</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Vanilys</t>
+          <t>no_me_la_calo</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>16</v>
+        <v>1582</v>
       </c>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr">
         <is>
-          <t xml:space="preserve">.@realDonaldTrump  : You, sir, are the reason God created the middle finger.#ByeHannity #JoeBiden #Trump… https://t.co/7FsHgeINrG </t>
+          <t xml:space="preserve">RT @JUANdeITALIA: The president MR #TRUMP whatever HE may be in his imperfect behavior ... he is a patriot as well as a person who believes in GOD, t ... </t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t xml:space="preserve">.  : You, sir, are the reason God created the middle finger.
-#ByeHannity #JoeBiden #Trump… </t>
+          <t xml:space="preserve"> El presidente MR #TRUMP sea como sea EL en su conducta imperfecta ...es un patriota además de persona creyente en DIOS, t…</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t xml:space="preserve">.  : You, sir, are the reason God created the middle finger.#ByeHannity #JoeBiden #Trump…  </t>
+          <t xml:space="preserve"> The president MR #TRUMP whatever HE may be in his imperfect behavior ... he is a patriot as well as a person who believes in GOD, t ... </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Adjusted some parts on the analysis.html
</commit_message>
<xml_diff>
--- a/TwitterSentimentAnalyser/TSentimentAnalyser/static/raw_tweets.xlsx
+++ b/TwitterSentimentAnalyser/TSentimentAnalyser/static/raw_tweets.xlsx
@@ -506,60 +506,48 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>#Trump announced that he would fire #WilliamBarr.
-.
-.
-He reminds me of children ...😑
-#TrumpIsACriminal… https://t.co/1B51buQrc6</t>
+          <t>RT @CorentinSellin: 2) Dans la géographie des élus républicains que je proposais il y a 3 semaines en fonction de la proximité avec #Trump…</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1.338856399380623e+18</v>
+        <v>1.338875729090646e+18</v>
       </c>
       <c r="D2" t="n">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>44180.61128472222</v>
+        <v>44180.66461805555</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>fr</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>1.273713204242395e+18</v>
+        <v>561047377</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Ashleysullivan_</t>
+          <t>cmtehcip</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>596</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Chicago</t>
-        </is>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
-          <t xml:space="preserve">#Trump announced that he would fire #WilliamBarr...He reminds me of children ...😑#TrumpIsACriminal… https://t.co/1B51buQrc6 </t>
+          <t xml:space="preserve">RT @CorentinSellin: 2) In the geography of Republican elected officials that I proposed 3 weeks ago depending on the proximity with # Trump… </t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t xml:space="preserve">#Trump announced that he would fire #WilliamBarr.
-.
-.
-He reminds me of children ...😑
-#TrumpIsACriminal… </t>
+          <t xml:space="preserve"> 2) Dans la géographie des élus républicains que je proposais il y a 3 semaines en fonction de la proximité avec #Trump…</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t xml:space="preserve">#Trump announced that he would fire #WilliamBarr...He reminds me of children ...😑#TrumpIsACriminal…  </t>
+          <t xml:space="preserve"> 2) In the geography of Republican elected officials that I proposed 3 weeks ago depending on the proximity with # Trump… </t>
         </is>
       </c>
     </row>
@@ -569,48 +557,52 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>RT @ManDessins: #COVID19 #USA #Trump #Dessin @Midilibre https://t.co/hv8DQwBzIc</t>
+          <t>RT @BeNosey: Sit tight stay tuned with our pinned tweet on this profile, our betfair WhatsApp group is already maxed out.... lots going on…</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1.3388563888234e+18</v>
+        <v>1.33887571669647e+18</v>
       </c>
       <c r="D3" t="n">
-        <v>79</v>
+        <v>139</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>44180.61125</v>
+        <v>44180.66458333333</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>und</t>
+          <t>en</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>604704562</v>
+        <v>1.047288807568151e+18</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>bonsoirmichel</t>
+          <t>imScottSigns</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>13262</v>
-      </c>
-      <c r="J3" t="inlineStr"/>
+        <v>10</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Kingwood, Houston</t>
+        </is>
+      </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @ManDessins: # COVID19 #USA #Trump #Dessin @Midilibre https://t.co/hv8DQwBzIc </t>
+          <t xml:space="preserve">RT @BeNosey: Sit tight stay tuned with our pinned tweet on this profile, our betfair WhatsApp group is already maxed out.... lots going on… </t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> #COVID19 #USA #Trump #Dessin  </t>
+          <t xml:space="preserve"> Sit tight stay tuned with our pinned tweet on this profile, our betfair WhatsApp group is already maxed out.... lots going on…</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> # COVID19 #USA #Trump #Dessin   </t>
+          <t xml:space="preserve"> Sit tight stay tuned with our pinned tweet on this profile, our betfair WhatsApp group is already maxed out.... lots going on… </t>
         </is>
       </c>
     </row>
@@ -620,19 +612,18 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>#Trump 
-this is the end
-Jim Morrison</t>
+          <t>The #turtle has finally spoken @senatemajldr congratulates @JoeBiden for #winning 
+First, #putin and now… https://t.co/rHgLG1YChL</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.338856381877604e+18</v>
+        <v>1.338875716692308e+18</v>
       </c>
       <c r="D4" t="n">
-        <v>37</v>
+        <v>130</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>44180.61122685186</v>
+        <v>44180.66458333333</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -640,36 +631,35 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>16604304</v>
+        <v>22511572</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>muehlenwind</t>
+          <t>jaypsalespro</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>2340</v>
+        <v>2358</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Sandstrand, Deutschland</t>
+          <t>New Jersey, USA</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t xml:space="preserve">#Trump this is the endJim Morrison </t>
+          <t xml:space="preserve">The #turtle has finally spoken @senatemajldr congratulates @JoeBiden for #winning First, #putin and now… https://t.co/rHgLG1YChL </t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>#Trump 
-this is the end
-Jim Morrison</t>
+          <t xml:space="preserve">The #turtle has finally spoken  congratulates  for #winning 
+First, #putin and now… </t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t xml:space="preserve">#Trump this is the endJim Morrison </t>
+          <t xml:space="preserve">The #turtle has finally spoken  congratulates  for #winning First, #putin and now…  </t>
         </is>
       </c>
     </row>
@@ -679,52 +669,54 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>@NotHoodlum Why is everyone so shocked? It’s the one promise #Trump kept - the entitled get more entitlement.… https://t.co/I95RVALzIQ</t>
+          <t>RT @robvegas: Einfach grandios. #Trump
+https://t.co/8dUuoYncOi</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1.338856364635009e+18</v>
+        <v>1.338875703803212e+18</v>
       </c>
       <c r="D5" t="n">
-        <v>134</v>
+        <v>62</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>44180.61118055556</v>
+        <v>44180.66454861111</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>de</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>757529364</v>
+        <v>496352617</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>MillieMinet</t>
+          <t>PeterLewis106</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>615</v>
+        <v>418</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>NPT</t>
+          <t xml:space="preserve">Andaluçía ۞ </t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t xml:space="preserve">@NotHoodlum Why is everyone so shocked? It’s the one promise #Trump kept - the entitled get more entitlement.… https://t.co/I95RVALzIQ </t>
+          <t xml:space="preserve">RT @robvegas: Simply terrific. #Trumphttps: //t.co/8dUuoYncOi </t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Why is everyone so shocked? It’s the one promise #Trump kept - the entitled get more entitlement.… </t>
+          <t xml:space="preserve"> Einfach grandios. #Trump
+</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Why is everyone so shocked? It’s the one promise #Trump kept - the entitled get more entitlement.…  </t>
+          <t xml:space="preserve"> Simply terrific. #Trumphttps: //t.co/8dUuoYncOi </t>
         </is>
       </c>
     </row>
@@ -734,52 +726,48 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>President Donald #Trump stands among Army cadets as he attends the annual Army-Navy collegiate football game in… https://t.co/P7nglPVrEb</t>
+          <t>RT @LuetzowQ: Schaut was der Präsident eben retweetet hat. Ich möchte jetzt nicht in der Haut des Gouverneurs von #Georgia stecken oder sei…</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1.338856361669616e+18</v>
+        <v>1.33887569712588e+18</v>
       </c>
       <c r="D6" t="n">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>44180.61118055556</v>
+        <v>44180.66452546296</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>de</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>8.42343300115927e+17</v>
+        <v>7.77783836717482e+17</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>pow_photos</t>
+          <t>danicita30081</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>806</v>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>Lebanon</t>
-        </is>
-      </c>
+        <v>493</v>
+      </c>
+      <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr">
         <is>
-          <t xml:space="preserve">President Donald #Trump stands among Army cadets as he attends the annual Army-Navy collegiate football game in… https://t.co/P7nglPVrEb </t>
+          <t xml:space="preserve">RT @LuetzowQ: Look what the president has just retweeted. I don't want to be in the shoes of the governor of #Georgia or be ... </t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t xml:space="preserve">President Donald #Trump stands among Army cadets as he attends the annual Army-Navy collegiate football game in… </t>
+          <t xml:space="preserve"> Schaut was der Präsident eben retweetet hat. Ich möchte jetzt nicht in der Haut des Gouverneurs von #Georgia stecken oder sei…</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t xml:space="preserve">President Donald #Trump stands among Army cadets as he attends the annual Army-Navy collegiate football game in…  </t>
+          <t xml:space="preserve"> Look what the president has just retweeted. I don't want to be in the shoes of the governor of #Georgia or be ... </t>
         </is>
       </c>
     </row>
@@ -789,54 +777,48 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>The electoral college has spoken. YOU LOST AGAIN. Perhaps #Trump is bad for America. 
-#ShutHimOut… https://t.co/1w7CuvK9Ri</t>
+          <t>@RND_de Es zeigt in welch bedauernswerten Zustand sich das politische System der USA nach 4 Jahren #Trump Wahnsinn… https://t.co/SDi3ZeeR7t</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1.338856349032178e+18</v>
+        <v>1.338875676636701e+18</v>
       </c>
       <c r="D7" t="n">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>44180.61114583333</v>
+        <v>44180.66447916667</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>de</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>267129243</v>
+        <v>2723803763</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>TarikuBogale</t>
+          <t>olli_mit_anker</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>5466</v>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>New York</t>
-        </is>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
-          <t xml:space="preserve">The electoral college has spoken. YOU LOST AGAIN. Perhaps #Trump is bad for America. #ShutHimOut… https://t.co/1w7CuvK9Ri </t>
+          <t xml:space="preserve">@RND_de It shows what a deplorable state the US political system is in after 4 years of #Trump madness ... https://t.co/SDi3ZeeR7t </t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t xml:space="preserve">The electoral college has spoken. YOU LOST AGAIN. Perhaps #Trump is bad for America. 
-#ShutHimOut… </t>
+          <t xml:space="preserve"> Es zeigt in welch bedauernswerten Zustand sich das politische System der USA nach 4 Jahren #Trump Wahnsinn… </t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t xml:space="preserve">The electoral college has spoken. YOU LOST AGAIN. Perhaps #Trump is bad for America. #ShutHimOut…  </t>
+          <t xml:space="preserve"> It shows what a deplorable state the US political system is in after 4 years of #Trump madness ...  </t>
         </is>
       </c>
     </row>
@@ -846,54 +828,48 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>RT @AlexdGtze: @washingtonpost Truth hurts
-#BidenVaccine #Trump https://t.co/1e8oIOxc5y</t>
+          <t>RT @CorentinSellin: TRES IMPORTANT: le patron, réélu cette année au Kentucky, de la majorité républicaine du Sénat, McConnell, reconnaît #B…</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1.338856347044033e+18</v>
+        <v>1.338875665341362e+18</v>
       </c>
       <c r="D8" t="n">
-        <v>87</v>
+        <v>140</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>44180.61113425926</v>
+        <v>44180.66444444445</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>fr</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>1.259356052635542e+18</v>
+        <v>561047377</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>JoeKing84576078</t>
+          <t>cmtehcip</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>511</v>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>Texas, USA</t>
-        </is>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @AlexdGtze: @washingtonpost Truth hurts#BidenVaccine #Trump https://t.co/1e8oIOxc5y </t>
+          <t xml:space="preserve">RT @CorentinSellin: VERY IMPORTANT: the boss, reelected this year in Kentucky, of the Senate Republican majority, McConnell, recognizes # B… </t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Truth hurts
-#BidenVaccine #Trump </t>
+          <t xml:space="preserve"> TRES IMPORTANT: le patron, réélu cette année au Kentucky, de la majorité républicaine du Sénat, McConnell, reconnaît #B…</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Truth hurts#BidenVaccine #Trump  </t>
+          <t xml:space="preserve"> VERY IMPORTANT: the boss, reelected this year in Kentucky, of the Senate Republican majority, McConnell, recognizes # B… </t>
         </is>
       </c>
     </row>
@@ -903,17 +879,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>@mkraju Strongly disagree with vacs for #Trump and #Pence. They have been advocating for super-spreading since the… https://t.co/Jm35wvOwH1</t>
+          <t>RT @DsOchoa: @POTUS 🗣 #Trump is an international embarrassment🤡</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1.338856345882096e+18</v>
+        <v>1.338875663877456e+18</v>
       </c>
       <c r="D9" t="n">
-        <v>139</v>
+        <v>63</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>44180.61113425926</v>
+        <v>44180.66444444445</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -921,30 +897,34 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>1.229178950347149e+18</v>
+        <v>9.928908583399055e+17</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>LAShake2</t>
+          <t>DsOchoa</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>7</v>
-      </c>
-      <c r="J9" t="inlineStr"/>
+        <v>4655</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>California, USA</t>
+        </is>
+      </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t xml:space="preserve">@mkraju Strongly disagree with vacs for #Trump and #Pence. They have been advocating for super-spreading since the… https://t.co/Jm35wvOwH1 </t>
+          <t xml:space="preserve">RT @DsOchoa: @POTUS 🗣 #Trump is an international embarrassment🤡 </t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Strongly disagree with vacs for #Trump and #Pence. They have been advocating for super-spreading since the… </t>
+          <t xml:space="preserve">  🗣 #Trump is an international embarrassment🤡</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Strongly disagree with vacs for #Trump and #Pence. They have been advocating for super-spreading since the…  </t>
+          <t xml:space="preserve">  🗣 #Trump is an international embarrassment🤡 </t>
         </is>
       </c>
     </row>
@@ -954,17 +934,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>@JoeBiden We all know you cheated. The sad thing is, YOU probably don’t know you cheated. The audacity to write thi… https://t.co/wXz7eT8rMF</t>
+          <t>If @msnbc and @cnn are worried about a post-#Trump reality, shouldn’t @twitter too?  I, for one, hope to spend a lot less time here. You?</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1.338856318673809e+18</v>
+        <v>1.33887562414497e+18</v>
       </c>
       <c r="D10" t="n">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>44180.61105324074</v>
+        <v>44180.6643287037</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -972,34 +952,34 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>1.298013110691758e+18</v>
+        <v>26076682</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>JiruJoshua</t>
+          <t>MRintouch</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>17</v>
+        <v>1195</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Madison, WI</t>
+          <t>Cambridge, MA</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t xml:space="preserve">@JoeBiden We all know you cheated. The sad thing is, YOU probably don’t know you cheated. The audacity to write thi… https://t.co/wXz7eT8rMF </t>
+          <t xml:space="preserve">If @msnbc and @cnn are worried about a post-#Trump reality, shouldn’t @twitter too?  I, for one, hope to spend a lot less time here. You? </t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> We all know you cheated. The sad thing is, YOU probably don’t know you cheated. The audacity to write thi… </t>
+          <t>If  and  are worried about a post-#Trump reality, shouldn’t  too?  I, for one, hope to spend a lot less time here. You?</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> We all know you cheated. The sad thing is, YOU probably don’t know you cheated. The audacity to write thi…  </t>
+          <t xml:space="preserve">If  and  are worried about a post-#Trump reality, shouldn’t  too?  I, for one, hope to spend a lot less time here. You? </t>
         </is>
       </c>
     </row>
@@ -1009,48 +989,52 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>RT @JUANdeITALIA: El presidente MR #TRUMP sea como sea EL en su conducta imperfecta ...es un patriota además de persona creyente en DIOS, t…</t>
+          <t>@POTUS 🗣 #Trump is an international embarrassment🤡 https://t.co/FSOnEBRkes</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1.338856311044321e+18</v>
+        <v>1.338875623456997e+18</v>
       </c>
       <c r="D11" t="n">
-        <v>140</v>
+        <v>74</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>44180.61103009259</v>
+        <v>44180.6643287037</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>es</t>
+          <t>en</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>353243516</v>
+        <v>9.928908583399055e+17</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>no_me_la_calo</t>
+          <t>DsOchoa</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>1582</v>
-      </c>
-      <c r="J11" t="inlineStr"/>
+        <v>4655</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>California, USA</t>
+        </is>
+      </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @JUANdeITALIA: The president MR #TRUMP whatever HE may be in his imperfect behavior ... he is a patriot as well as a person who believes in GOD, t ... </t>
+          <t xml:space="preserve">@POTUS 🗣 #Trump is an international embarrassment🤡 https://t.co/FSOnEBRkes </t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> El presidente MR #TRUMP sea como sea EL en su conducta imperfecta ...es un patriota además de persona creyente en DIOS, t…</t>
+          <t xml:space="preserve"> 🗣 #Trump is an international embarrassment🤡 </t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The president MR #TRUMP whatever HE may be in his imperfect behavior ... he is a patriot as well as a person who believes in GOD, t ... </t>
+          <t xml:space="preserve"> 🗣 #Trump is an international embarrassment🤡  </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Zoom meeting changes Edited descriptions, minor changes to visualization, removed unnecessary code parts
</commit_message>
<xml_diff>
--- a/TwitterSentimentAnalyser/TSentimentAnalyser/static/raw_tweets.xlsx
+++ b/TwitterSentimentAnalyser/TSentimentAnalyser/static/raw_tweets.xlsx
@@ -506,48 +506,48 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>RT @CorentinSellin: 2) Dans la géographie des élus républicains que je proposais il y a 3 semaines en fonction de la proximité avec #Trump…</t>
+          <t>RT @MikeThePlumbe10: 🚨ACCORDING TO A BRAND NEW #RASMUSSEN POLL EVEN 30 #PERCENT OF #DEMS THINK OUR NOV 3RD #ELECTION WAS #FRAUDULENT‼️WONDE…</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1.338875729090646e+18</v>
+        <v>1.338899682798563e+18</v>
       </c>
       <c r="D2" t="n">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>44180.66461805555</v>
+        <v>44180.7307175926</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>fr</t>
+          <t>en</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>561047377</v>
+        <v>1.206935907036795e+18</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>cmtehcip</t>
+          <t>MikeThePlumbe10</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>187</v>
+        <v>9132</v>
       </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @CorentinSellin: 2) In the geography of Republican elected officials that I proposed 3 weeks ago depending on the proximity with # Trump… </t>
+          <t xml:space="preserve">RT @MikeThePlumbe10: 🚨ACCORDING TO A BRAND NEW #RASMUSSEN POLL EVEN 30 #PERCENT OF #DEMS THINK OUR NOV 3RD #ELECTION WAS #FRAUDULENT‼️WONDE… </t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 2) Dans la géographie des élus républicains que je proposais il y a 3 semaines en fonction de la proximité avec #Trump…</t>
+          <t xml:space="preserve"> 🚨ACCORDING TO A BRAND NEW #RASMUSSEN POLL EVEN 30 #PERCENT OF #DEMS THINK OUR NOV 3RD #ELECTION WAS #FRAUDULENT‼️WONDE…</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 2) In the geography of Republican elected officials that I proposed 3 weeks ago depending on the proximity with # Trump… </t>
+          <t xml:space="preserve"> 🚨ACCORDING TO A BRAND NEW #RASMUSSEN POLL EVEN 30 #PERCENT OF #DEMS THINK OUR NOV 3RD #ELECTION WAS #FRAUDULENT‼️WONDE… </t>
         </is>
       </c>
     </row>
@@ -557,17 +557,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>RT @BeNosey: Sit tight stay tuned with our pinned tweet on this profile, our betfair WhatsApp group is already maxed out.... lots going on…</t>
+          <t>RT @truth2power2ppl: In the last 3 weeks, @realDonaldTrump has lost more legal cases than Hamilton Burger did during 9 seasons of Perry Mas…</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1.33887571669647e+18</v>
+        <v>1.338899673277293e+18</v>
       </c>
       <c r="D3" t="n">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>44180.66458333333</v>
+        <v>44180.73069444444</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -575,34 +575,30 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>1.047288807568151e+18</v>
+        <v>2714877872</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>imScottSigns</t>
+          <t>truth2power2ppl</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>10</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Kingwood, Houston</t>
-        </is>
-      </c>
+        <v>2785</v>
+      </c>
+      <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @BeNosey: Sit tight stay tuned with our pinned tweet on this profile, our betfair WhatsApp group is already maxed out.... lots going on… </t>
+          <t xml:space="preserve">RT @truth2power2ppl: In the last 3 weeks, @realDonaldTrump has lost more legal cases than Hamilton Burger did during 9 seasons of Perry Mas… </t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Sit tight stay tuned with our pinned tweet on this profile, our betfair WhatsApp group is already maxed out.... lots going on…</t>
+          <t xml:space="preserve"> In the last 3 weeks,  has lost more legal cases than Hamilton Burger did during 9 seasons of Perry Mas…</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Sit tight stay tuned with our pinned tweet on this profile, our betfair WhatsApp group is already maxed out.... lots going on… </t>
+          <t xml:space="preserve"> In the last 3 weeks,  has lost more legal cases than Hamilton Burger did during 9 seasons of Perry Mas… </t>
         </is>
       </c>
     </row>
@@ -612,54 +608,48 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>The #turtle has finally spoken @senatemajldr congratulates @JoeBiden for #winning 
-First, #putin and now… https://t.co/rHgLG1YChL</t>
+          <t>@Myname04734338 @CelineJullie @CorentinSellin @CorentinSellin qui interdit déjà à tout le monde de répondre à ses t… https://t.co/sQdbQyym9t</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.338875716692308e+18</v>
+        <v>1.338899663429186e+18</v>
       </c>
       <c r="D4" t="n">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>44180.66458333333</v>
+        <v>44180.73065972222</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>fr</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>22511572</v>
+        <v>2185004262</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>jaypsalespro</t>
+          <t>badsquirrell</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>2358</v>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>New Jersey, USA</t>
-        </is>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr">
         <is>
-          <t xml:space="preserve">The #turtle has finally spoken @senatemajldr congratulates @JoeBiden for #winning First, #putin and now… https://t.co/rHgLG1YChL </t>
+          <t xml:space="preserve">@ Myname04734338 @CelineJullie @CorentinSellin @CorentinSellin who already forbids everyone to answer their t ... https://t.co/sQdbQyym9t </t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t xml:space="preserve">The #turtle has finally spoken  congratulates  for #winning 
-First, #putin and now… </t>
+          <t xml:space="preserve">    qui interdit déjà à tout le monde de répondre à ses t… </t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t xml:space="preserve">The #turtle has finally spoken  congratulates  for #winning First, #putin and now…  </t>
+          <t xml:space="preserve"> Myname04734338 CelineJullie CorentinSellin CorentinSellin who already forbids everyone to answer their t ...  </t>
         </is>
       </c>
     </row>
@@ -669,54 +659,56 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>RT @robvegas: Einfach grandios. #Trump
-https://t.co/8dUuoYncOi</t>
+          <t>RT @dennis0805a: @realDonaldTrump THE 2020 ELECTION:
+@JoeBiden crushed #Trump in Popular Vote 😀
+@JoeBiden crushed #Trump in Electoral Col…</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1.338875703803212e+18</v>
+        <v>1.338899652104475e+18</v>
       </c>
       <c r="D5" t="n">
-        <v>62</v>
+        <v>140</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>44180.66454861111</v>
+        <v>44180.73063657407</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>de</t>
+          <t>en</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>496352617</v>
+        <v>229075545</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>PeterLewis106</t>
+          <t>sleddogwatchdog</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>418</v>
+        <v>6848</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Andaluçía ۞ </t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @robvegas: Simply terrific. #Trumphttps: //t.co/8dUuoYncOi </t>
+          <t xml:space="preserve">RT @dennis0805a: @realDonaldTrump THE 2020 ELECTION:@JoeBiden crushed #Trump in Popular Vote 😀@JoeBiden crushed #Trump in Electoral Col… </t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Einfach grandios. #Trump
-</t>
+          <t xml:space="preserve">  THE 2020 ELECTION:
+ crushed #Trump in Popular Vote 😀
+ crushed #Trump in Electoral Col…</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Simply terrific. #Trumphttps: //t.co/8dUuoYncOi </t>
+          <t xml:space="preserve">  THE 2020 ELECTION: crushed #Trump in Popular Vote 😀 crushed #Trump in Electoral Col… </t>
         </is>
       </c>
     </row>
@@ -726,48 +718,48 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>RT @LuetzowQ: Schaut was der Präsident eben retweetet hat. Ich möchte jetzt nicht in der Haut des Gouverneurs von #Georgia stecken oder sei…</t>
+          <t>🚨ACCORDING TO A BRAND NEW #RASMUSSEN POLL EVEN 30 #PERCENT OF #DEMS THINK OUR NOV 3RD #ELECTION WAS #FRAUDULENT‼️WO… https://t.co/S8SI7d6wK1</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1.33887569712588e+18</v>
+        <v>1.338899644886241e+18</v>
       </c>
       <c r="D6" t="n">
         <v>140</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>44180.66452546296</v>
+        <v>44180.73061342593</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>de</t>
+          <t>en</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>7.77783836717482e+17</v>
+        <v>1.206935907036795e+18</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>danicita30081</t>
+          <t>MikeThePlumbe10</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>493</v>
+        <v>9132</v>
       </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @LuetzowQ: Look what the president has just retweeted. I don't want to be in the shoes of the governor of #Georgia or be ... </t>
+          <t xml:space="preserve">🚨ACCORDING TO A BRAND NEW #RASMUSSEN POLL EVEN 30 #PERCENT OF #DEMS THINK OUR NOV 3RD #ELECTION WAS #FRAUDULENT‼️WO… https://t.co/S8SI7d6wK1 </t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Schaut was der Präsident eben retweetet hat. Ich möchte jetzt nicht in der Haut des Gouverneurs von #Georgia stecken oder sei…</t>
+          <t xml:space="preserve">🚨ACCORDING TO A BRAND NEW #RASMUSSEN POLL EVEN 30 #PERCENT OF #DEMS THINK OUR NOV 3RD #ELECTION WAS #FRAUDULENT‼️WO… </t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Look what the president has just retweeted. I don't want to be in the shoes of the governor of #Georgia or be ... </t>
+          <t xml:space="preserve">🚨ACCORDING TO A BRAND NEW #RASMUSSEN POLL EVEN 30 #PERCENT OF #DEMS THINK OUR NOV 3RD #ELECTION WAS #FRAUDULENT‼️WO…  </t>
         </is>
       </c>
     </row>
@@ -777,48 +769,52 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>@RND_de Es zeigt in welch bedauernswerten Zustand sich das politische System der USA nach 4 Jahren #Trump Wahnsinn… https://t.co/SDi3ZeeR7t</t>
+          <t>RT @EJDionne: It was right and necessary for  @JoeBiden to take on the outrageous, anti-democratic lawsuit filed by Texas and to push back…</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1.338875676636701e+18</v>
+        <v>1.338899627391689e+18</v>
       </c>
       <c r="D7" t="n">
         <v>139</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>44180.66447916667</v>
+        <v>44180.73056712963</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>de</t>
+          <t>en</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>2723803763</v>
+        <v>340730132</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>olli_mit_anker</t>
+          <t>Dr_Markie_Twist</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>196</v>
-      </c>
-      <c r="J7" t="inlineStr"/>
+        <v>1176</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Las Vegas, NV</t>
+        </is>
+      </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t xml:space="preserve">@RND_de It shows what a deplorable state the US political system is in after 4 years of #Trump madness ... https://t.co/SDi3ZeeR7t </t>
+          <t xml:space="preserve">RT @EJDionne: It was right and necessary for  @JoeBiden to take on the outrageous, anti-democratic lawsuit filed by Texas and to push back… </t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Es zeigt in welch bedauernswerten Zustand sich das politische System der USA nach 4 Jahren #Trump Wahnsinn… </t>
+          <t xml:space="preserve"> It was right and necessary for   to take on the outrageous, anti-democratic lawsuit filed by Texas and to push back…</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> It shows what a deplorable state the US political system is in after 4 years of #Trump madness ...  </t>
+          <t xml:space="preserve"> It was right and necessary for   to take on the outrageous, anti-democratic lawsuit filed by Texas and to push back… </t>
         </is>
       </c>
     </row>
@@ -828,48 +824,48 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>RT @CorentinSellin: TRES IMPORTANT: le patron, réélu cette année au Kentucky, de la majorité républicaine du Sénat, McConnell, reconnaît #B…</t>
+          <t>@Harlan By 80 million #americans who throw up every morning knowing he’s still #potus. Btw, #trump just called, his… https://t.co/HnjSBpqVPh</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1.338875665341362e+18</v>
+        <v>1.338899623222579e+18</v>
       </c>
       <c r="D8" t="n">
         <v>140</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>44180.66444444445</v>
+        <v>44180.73055555556</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>fr</t>
+          <t>en</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>561047377</v>
+        <v>1.22813057475953e+18</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>cmtehcip</t>
+          <t>GarissonJim</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>187</v>
+        <v>1</v>
       </c>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @CorentinSellin: VERY IMPORTANT: the boss, reelected this year in Kentucky, of the Senate Republican majority, McConnell, recognizes # B… </t>
+          <t xml:space="preserve">@Harlan By 80 million #americans who throw up every morning knowing he’s still #potus. Btw, #trump just called, his… https://t.co/HnjSBpqVPh </t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> TRES IMPORTANT: le patron, réélu cette année au Kentucky, de la majorité républicaine du Sénat, McConnell, reconnaît #B…</t>
+          <t xml:space="preserve"> By 80 million #americans who throw up every morning knowing he’s still #potus. Btw, #trump just called, his… </t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> VERY IMPORTANT: the boss, reelected this year in Kentucky, of the Senate Republican majority, McConnell, recognizes # B… </t>
+          <t xml:space="preserve"> By 80 million #americans who throw up every morning knowing he’s still #potus. Btw, #trump just called, his…  </t>
         </is>
       </c>
     </row>
@@ -879,17 +875,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>RT @DsOchoa: @POTUS 🗣 #Trump is an international embarrassment🤡</t>
+          <t>@jimsciutto They didn’t ignore it #Trump got a big loan to payoff so he left the keys in the ignition on purpose -</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1.338875663877456e+18</v>
+        <v>1.338899613147787e+18</v>
       </c>
       <c r="D9" t="n">
-        <v>63</v>
+        <v>114</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>44180.66444444445</v>
+        <v>44180.73052083333</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -897,34 +893,34 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>9.928908583399055e+17</v>
+        <v>8.859419104890552e+17</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>DsOchoa</t>
+          <t>TGEE21</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>4655</v>
+        <v>299</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>California, USA</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @DsOchoa: @POTUS 🗣 #Trump is an international embarrassment🤡 </t>
+          <t xml:space="preserve">@jimsciutto They didn’t ignore it #Trump got a big loan to payoff so he left the keys in the ignition on purpose - </t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t xml:space="preserve">  🗣 #Trump is an international embarrassment🤡</t>
+          <t xml:space="preserve"> They didn’t ignore it #Trump got a big loan to payoff so he left the keys in the ignition on purpose -</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t xml:space="preserve">  🗣 #Trump is an international embarrassment🤡 </t>
+          <t xml:space="preserve"> They didn’t ignore it #Trump got a big loan to payoff so he left the keys in the ignition on purpose - </t>
         </is>
       </c>
     </row>
@@ -934,17 +930,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>If @msnbc and @cnn are worried about a post-#Trump reality, shouldn’t @twitter too?  I, for one, hope to spend a lot less time here. You?</t>
+          <t>RT @changefromthei1: #Trump and his daughter @IvankaTrump relationship has always had blurred lines. https://t.co/5G6Qg449dO</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1.33887562414497e+18</v>
+        <v>1.338899561960575e+18</v>
       </c>
       <c r="D10" t="n">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>44180.6643287037</v>
+        <v>44180.73038194444</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -952,34 +948,34 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>26076682</v>
+        <v>1.333393595634749e+18</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>MRintouch</t>
+          <t>caster_midnight</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>1195</v>
+        <v>14</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Cambridge, MA</t>
+          <t>the world</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t xml:space="preserve">If @msnbc and @cnn are worried about a post-#Trump reality, shouldn’t @twitter too?  I, for one, hope to spend a lot less time here. You? </t>
+          <t xml:space="preserve">RT @changefromthei1: #Trump and his daughter @IvankaTrump relationship has always had blurred lines. https://t.co/5G6Qg449dO </t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>If  and  are worried about a post-#Trump reality, shouldn’t  too?  I, for one, hope to spend a lot less time here. You?</t>
+          <t xml:space="preserve"> #Trump and his daughter  relationship has always had blurred lines. </t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t xml:space="preserve">If  and  are worried about a post-#Trump reality, shouldn’t  too?  I, for one, hope to spend a lot less time here. You? </t>
+          <t xml:space="preserve"> #Trump and his daughter  relationship has always had blurred lines.  </t>
         </is>
       </c>
     </row>
@@ -989,52 +985,60 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>@POTUS 🗣 #Trump is an international embarrassment🤡 https://t.co/FSOnEBRkes</t>
+          <t>RT @Toprak__46: #2020ninKaybedeni
+#Trump #CHPdeZincirlemeTaciz #Macron #SuudHanedanı 
+#YorumaGerekYok 
+#Degersiz 
+#çöplük https://t.co/7Mxl…</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1.338875623456997e+18</v>
+        <v>1.338899550396965e+18</v>
       </c>
       <c r="D11" t="n">
-        <v>74</v>
+        <v>140</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>44180.6643287037</v>
+        <v>44180.7303587963</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>und</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>9.928908583399055e+17</v>
+        <v>4458266847</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>DsOchoa</t>
+          <t>rte_tim_</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>4655</v>
+        <v>4495</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>California, USA</t>
+          <t xml:space="preserve">Mersin Malatya </t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t xml:space="preserve">@POTUS 🗣 #Trump is an international embarrassment🤡 https://t.co/FSOnEBRkes </t>
+          <t xml:space="preserve">RT @ Toprak__46: # 2020ninKaybedeni # Trump #CHPdeZincirlemeAbuse #Macron # SuudHanedanı #YorumaGerekYok #Degersiz # dump https://t.co/7Mxl… </t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 🗣 #Trump is an international embarrassment🤡 </t>
+          <t xml:space="preserve"> #2020ninKaybedeni
+#Trump #CHPdeZincirlemeTaciz #Macron #SuudHanedanı 
+#YorumaGerekYok 
+#Degersiz 
+#çöplük …</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 🗣 #Trump is an international embarrassment🤡  </t>
+          <t xml:space="preserve">RT  Toprak__46: # 2020ninKaybedeni # Trump #CHPdeZincirlemeAbuse #Macron # SuudHanedanı #YorumaGerekYok #Degersiz # dump … </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Pathing for Excel file should now be fixed
</commit_message>
<xml_diff>
--- a/TwitterSentimentAnalyser/TSentimentAnalyser/static/raw_tweets.xlsx
+++ b/TwitterSentimentAnalyser/TSentimentAnalyser/static/raw_tweets.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,17 +506,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>RT @MikeThePlumbe10: 🚨ACCORDING TO A BRAND NEW #RASMUSSEN POLL EVEN 30 #PERCENT OF #DEMS THINK OUR NOV 3RD #ELECTION WAS #FRAUDULENT‼️WONDE…</t>
+          <t>RT @kk131066: PATRIOTISM
+is not about how long
+you hold on to a lie,
+but how quickly you can
+get rid of it to save your country
+#Hypocrisy…</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1.338899682798563e+18</v>
+        <v>1.339116294600352e+18</v>
       </c>
       <c r="D2" t="n">
         <v>140</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>44180.7307175926</v>
+        <v>44181.32844907408</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -524,30 +529,39 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>1.206935907036795e+18</v>
+        <v>8.22989712692482e+17</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>MikeThePlumbe10</t>
+          <t>ResistOrganize</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>9132</v>
-      </c>
-      <c r="J2" t="inlineStr"/>
+        <v>5202</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Washington, DC</t>
+        </is>
+      </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @MikeThePlumbe10: 🚨ACCORDING TO A BRAND NEW #RASMUSSEN POLL EVEN 30 #PERCENT OF #DEMS THINK OUR NOV 3RD #ELECTION WAS #FRAUDULENT‼️WONDE… </t>
+          <t xml:space="preserve">RT @kk131066: PATRIOTISM is not about how long you hold onto a lie,but how quickly you canget rid of it to save your country#Hypocrisy… </t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 🚨ACCORDING TO A BRAND NEW #RASMUSSEN POLL EVEN 30 #PERCENT OF #DEMS THINK OUR NOV 3RD #ELECTION WAS #FRAUDULENT‼️WONDE…</t>
+          <t xml:space="preserve"> PATRIOTISM
+is not about how long
+you hold on to a lie,
+but how quickly you can
+get rid of it to save your country
+#Hypocrisy…</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 🚨ACCORDING TO A BRAND NEW #RASMUSSEN POLL EVEN 30 #PERCENT OF #DEMS THINK OUR NOV 3RD #ELECTION WAS #FRAUDULENT‼️WONDE… </t>
+          <t xml:space="preserve"> PATRIOTISM is not about how long you hold onto a lie,but how quickly you canget rid of it to save your country#Hypocrisy… </t>
         </is>
       </c>
     </row>
@@ -557,48 +571,52 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>RT @truth2power2ppl: In the last 3 weeks, @realDonaldTrump has lost more legal cases than Hamilton Burger did during 9 seasons of Perry Mas…</t>
+          <t>A la ❓d'un anti #Trump sur sa "folie", l'une de mes abonnées répond : "Qui rapatrie les soldats, qui ne se soumet p… https://t.co/CZkkpIoFZl</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1.338899673277293e+18</v>
+        <v>1.339116293174288e+18</v>
       </c>
       <c r="D3" t="n">
         <v>140</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>44180.73069444444</v>
+        <v>44181.32844907408</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>fr</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>2714877872</v>
+        <v>1.334580217294303e+18</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>truth2power2ppl</t>
+          <t>1eDeCouverture</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>2785</v>
-      </c>
-      <c r="J3" t="inlineStr"/>
+        <v>288</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @truth2power2ppl: In the last 3 weeks, @realDonaldTrump has lost more legal cases than Hamilton Burger did during 9 seasons of Perry Mas… </t>
+          <t xml:space="preserve">Like an anti #Trump on his "madness", one of my subscribers replies: "Who repatriates soldiers, who does not submit ... https://t.co/CZkkpIoFZl </t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> In the last 3 weeks,  has lost more legal cases than Hamilton Burger did during 9 seasons of Perry Mas…</t>
+          <t xml:space="preserve">A la ❓d'un anti #Trump sur sa "folie", l'une de mes abonnées répond : "Qui rapatrie les soldats, qui ne se soumet p… </t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> In the last 3 weeks,  has lost more legal cases than Hamilton Burger did during 9 seasons of Perry Mas… </t>
+          <t xml:space="preserve">Like an anti #Trump on his "madness", one of my subscribers replies: "Who repatriates soldiers, who does not submit ...  </t>
         </is>
       </c>
     </row>
@@ -608,48 +626,54 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>@Myname04734338 @CelineJullie @CorentinSellin @CorentinSellin qui interdit déjà à tout le monde de répondre à ses t… https://t.co/sQdbQyym9t</t>
+          <t>RT @news_ntd: White House press secretary responds to whether #Trump will acknowledge #Biden as #president-elect
+https://t.co/qPfBgigBJz</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.338899663429186e+18</v>
+        <v>1.33911628746145e+18</v>
       </c>
       <c r="D4" t="n">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>44180.73065972222</v>
+        <v>44181.3284375</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>fr</t>
+          <t>en</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>2185004262</v>
+        <v>28803556</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>badsquirrell</t>
+          <t>Syunrou</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>93</v>
-      </c>
-      <c r="J4" t="inlineStr"/>
+        <v>618</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Nagaoka-City, Niigata, Japan</t>
+        </is>
+      </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t xml:space="preserve">@ Myname04734338 @CelineJullie @CorentinSellin @CorentinSellin who already forbids everyone to answer their t ... https://t.co/sQdbQyym9t </t>
+          <t xml:space="preserve">RT @news_ntd: White House press secretary responds to whether #Trump will acknowledge #Biden as #president-electhttps://t.co/qPfBgigBJz </t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t xml:space="preserve">    qui interdit déjà à tout le monde de répondre à ses t… </t>
+          <t xml:space="preserve"> White House press secretary responds to whether #Trump will acknowledge #Biden as #president-elect
+</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Myname04734338 CelineJullie CorentinSellin CorentinSellin who already forbids everyone to answer their t ...  </t>
+          <t xml:space="preserve"> White House press secretary responds to whether #Trump will acknowledge #Biden as #president-elect </t>
         </is>
       </c>
     </row>
@@ -659,19 +683,18 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>RT @dennis0805a: @realDonaldTrump THE 2020 ELECTION:
-@JoeBiden crushed #Trump in Popular Vote 😀
-@JoeBiden crushed #Trump in Electoral Col…</t>
+          <t>I may just a tiny dust to President Trump as a foriener,
+My donation is unacceptable to #Trump, but my heart for Tr… https://t.co/ndIpvevYtJ</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1.338899652104475e+18</v>
+        <v>1.339116281253917e+18</v>
       </c>
       <c r="D5" t="n">
         <v>140</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>44180.73063657407</v>
+        <v>44181.32841435185</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -679,36 +702,31 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>229075545</v>
+        <v>1.321640627977613e+18</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>sleddogwatchdog</t>
+          <t>AdeleTWin</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>6848</v>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Canada</t>
-        </is>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @dennis0805a: @realDonaldTrump THE 2020 ELECTION:@JoeBiden crushed #Trump in Popular Vote 😀@JoeBiden crushed #Trump in Electoral Col… </t>
+          <t xml:space="preserve">I may just a tiny dust to President Trump as a foreigner,My donation is unacceptable to #Trump, but my heart for Tr… https://t.co/ndIpvevYtJ </t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t xml:space="preserve">  THE 2020 ELECTION:
- crushed #Trump in Popular Vote 😀
- crushed #Trump in Electoral Col…</t>
+          <t xml:space="preserve">I may just a tiny dust to President Trump as a foriener,
+My donation is unacceptable to #Trump, but my heart for Tr… </t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t xml:space="preserve">  THE 2020 ELECTION: crushed #Trump in Popular Vote 😀 crushed #Trump in Electoral Col… </t>
+          <t xml:space="preserve">I may just a tiny dust to President Trump as a foreigner,My donation is unacceptable to #Trump, but my heart for Tr…  </t>
         </is>
       </c>
     </row>
@@ -718,327 +736,48 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>🚨ACCORDING TO A BRAND NEW #RASMUSSEN POLL EVEN 30 #PERCENT OF #DEMS THINK OUR NOV 3RD #ELECTION WAS #FRAUDULENT‼️WO… https://t.co/S8SI7d6wK1</t>
+          <t>RT @gDesFaits: Biden en Géorgie aujourd’hui ! Et on veut nous faire croire que ça va être le nouveau président et qu’il a obtenu 80 million…</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1.338899644886241e+18</v>
+        <v>1.33911626612095e+18</v>
       </c>
       <c r="D6" t="n">
         <v>140</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>44180.73061342593</v>
+        <v>44181.32837962963</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>fr</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>1.206935907036795e+18</v>
+        <v>310473863</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>MikeThePlumbe10</t>
+          <t>frombergers</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>9132</v>
+        <v>626</v>
       </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr">
         <is>
-          <t xml:space="preserve">🚨ACCORDING TO A BRAND NEW #RASMUSSEN POLL EVEN 30 #PERCENT OF #DEMS THINK OUR NOV 3RD #ELECTION WAS #FRAUDULENT‼️WO… https://t.co/S8SI7d6wK1 </t>
+          <t xml:space="preserve">RT @gDesFaits: Biden in Georgia today! And they want us to believe that this is going to be the new president and that he got 80 million ... </t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t xml:space="preserve">🚨ACCORDING TO A BRAND NEW #RASMUSSEN POLL EVEN 30 #PERCENT OF #DEMS THINK OUR NOV 3RD #ELECTION WAS #FRAUDULENT‼️WO… </t>
+          <t xml:space="preserve"> Biden en Géorgie aujourd’hui ! Et on veut nous faire croire que ça va être le nouveau président et qu’il a obtenu 80 million…</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t xml:space="preserve">🚨ACCORDING TO A BRAND NEW #RASMUSSEN POLL EVEN 30 #PERCENT OF #DEMS THINK OUR NOV 3RD #ELECTION WAS #FRAUDULENT‼️WO…  </t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>RT @EJDionne: It was right and necessary for  @JoeBiden to take on the outrageous, anti-democratic lawsuit filed by Texas and to push back…</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>1.338899627391689e+18</v>
-      </c>
-      <c r="D7" t="n">
-        <v>139</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>44180.73056712963</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
-        <v>340730132</v>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Dr_Markie_Twist</t>
-        </is>
-      </c>
-      <c r="I7" t="n">
-        <v>1176</v>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Las Vegas, NV</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">RT @EJDionne: It was right and necessary for  @JoeBiden to take on the outrageous, anti-democratic lawsuit filed by Texas and to push back… </t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> It was right and necessary for   to take on the outrageous, anti-democratic lawsuit filed by Texas and to push back…</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> It was right and necessary for   to take on the outrageous, anti-democratic lawsuit filed by Texas and to push back… </t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>@Harlan By 80 million #americans who throw up every morning knowing he’s still #potus. Btw, #trump just called, his… https://t.co/HnjSBpqVPh</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>1.338899623222579e+18</v>
-      </c>
-      <c r="D8" t="n">
-        <v>140</v>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>44180.73055555556</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
-        <v>1.22813057475953e+18</v>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>GarissonJim</t>
-        </is>
-      </c>
-      <c r="I8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">@Harlan By 80 million #americans who throw up every morning knowing he’s still #potus. Btw, #trump just called, his… https://t.co/HnjSBpqVPh </t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> By 80 million #americans who throw up every morning knowing he’s still #potus. Btw, #trump just called, his… </t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> By 80 million #americans who throw up every morning knowing he’s still #potus. Btw, #trump just called, his…  </t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>@jimsciutto They didn’t ignore it #Trump got a big loan to payoff so he left the keys in the ignition on purpose -</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>1.338899613147787e+18</v>
-      </c>
-      <c r="D9" t="n">
-        <v>114</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>44180.73052083333</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="G9" t="n">
-        <v>8.859419104890552e+17</v>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>TGEE21</t>
-        </is>
-      </c>
-      <c r="I9" t="n">
-        <v>299</v>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>United States</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">@jimsciutto They didn’t ignore it #Trump got a big loan to payoff so he left the keys in the ignition on purpose - </t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> They didn’t ignore it #Trump got a big loan to payoff so he left the keys in the ignition on purpose -</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> They didn’t ignore it #Trump got a big loan to payoff so he left the keys in the ignition on purpose - </t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>RT @changefromthei1: #Trump and his daughter @IvankaTrump relationship has always had blurred lines. https://t.co/5G6Qg449dO</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>1.338899561960575e+18</v>
-      </c>
-      <c r="D10" t="n">
-        <v>124</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>44180.73038194444</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="G10" t="n">
-        <v>1.333393595634749e+18</v>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>caster_midnight</t>
-        </is>
-      </c>
-      <c r="I10" t="n">
-        <v>14</v>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>the world</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">RT @changefromthei1: #Trump and his daughter @IvankaTrump relationship has always had blurred lines. https://t.co/5G6Qg449dO </t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> #Trump and his daughter  relationship has always had blurred lines. </t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> #Trump and his daughter  relationship has always had blurred lines.  </t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>RT @Toprak__46: #2020ninKaybedeni
-#Trump #CHPdeZincirlemeTaciz #Macron #SuudHanedanı 
-#YorumaGerekYok 
-#Degersiz 
-#çöplük https://t.co/7Mxl…</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>1.338899550396965e+18</v>
-      </c>
-      <c r="D11" t="n">
-        <v>140</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>44180.7303587963</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>und</t>
-        </is>
-      </c>
-      <c r="G11" t="n">
-        <v>4458266847</v>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>rte_tim_</t>
-        </is>
-      </c>
-      <c r="I11" t="n">
-        <v>4495</v>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Mersin Malatya </t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">RT @ Toprak__46: # 2020ninKaybedeni # Trump #CHPdeZincirlemeAbuse #Macron # SuudHanedanı #YorumaGerekYok #Degersiz # dump https://t.co/7Mxl… </t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> #2020ninKaybedeni
-#Trump #CHPdeZincirlemeTaciz #Macron #SuudHanedanı 
-#YorumaGerekYok 
-#Degersiz 
-#çöplük …</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">RT  Toprak__46: # 2020ninKaybedeni # Trump #CHPdeZincirlemeAbuse #Macron # SuudHanedanı #YorumaGerekYok #Degersiz # dump … </t>
+          <t xml:space="preserve"> Biden in Georgia today! And they want us to believe that this is going to be the new president and that he got 80 million ... </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed sizes for boxplot and distribution on analysis.html
</commit_message>
<xml_diff>
--- a/TwitterSentimentAnalyser/TSentimentAnalyser/static/raw_tweets.xlsx
+++ b/TwitterSentimentAnalyser/TSentimentAnalyser/static/raw_tweets.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,6 +499,11 @@
           <t>cleaned_english_tweets</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>html_ready_tweets</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -506,22 +511,19 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>RT @kk131066: PATRIOTISM
-is not about how long
-you hold on to a lie,
-but how quickly you can
-get rid of it to save your country
-#Hypocrisy…</t>
+          <t>RT @SandraSentinel: 8th commandment from God. "Thou Shall Not Steal"
+Our voting process has been stolen.
+Our right to have the president w…</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1.339116294600352e+18</v>
+        <v>1.339123251994247e+18</v>
       </c>
       <c r="D2" t="n">
         <v>140</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>44181.32844907408</v>
+        <v>44181.34765046297</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -529,39 +531,35 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>8.22989712692482e+17</v>
+        <v>1.22176409109144e+18</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>ResistOrganize</t>
+          <t>CHUGGER50357510</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>5202</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Washington, DC</t>
-        </is>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @kk131066: PATRIOTISM is not about how long you hold onto a lie,but how quickly you canget rid of it to save your country#Hypocrisy… </t>
+          <t xml:space="preserve">RT @SandraSentinel: 8th commandment from God. "Thou Shall Not Steal"Our voting process has been stolen.Our right to have the president w… </t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PATRIOTISM
-is not about how long
-you hold on to a lie,
-but how quickly you can
-get rid of it to save your country
-#Hypocrisy…</t>
+          <t xml:space="preserve"> 8th commandment from God. "Thou Shall Not Steal"  Our voting process has been stolen. Our right to have the president w…</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PATRIOTISM is not about how long you hold onto a lie,but how quickly you canget rid of it to save your country#Hypocrisy… </t>
+          <t xml:space="preserve"> 8th commandment from God. "Thou Shall Not Steal"Our voting process has been stolen.Our right to have the president w… </t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RT @SandraSentinel: 8th commandment from God. "Thou Shall Not Steal"Our voting process has been stolen.Our right to have the president w… </t>
         </is>
       </c>
     </row>
@@ -571,52 +569,53 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>A la ❓d'un anti #Trump sur sa "folie", l'une de mes abonnées répond : "Qui rapatrie les soldats, qui ne se soumet p… https://t.co/CZkkpIoFZl</t>
+          <t>@EdRaposo1 Não existe absolutamente nada confirmado. Ao contrário do que a mídia veicula por aí. QUEM DECIDE É O MI… https://t.co/e148rLNWg2</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1.339116293174288e+18</v>
+        <v>1.339123246055231e+18</v>
       </c>
       <c r="D3" t="n">
         <v>140</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>44181.32844907408</v>
+        <v>44181.34763888889</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>fr</t>
+          <t>pt</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>1.334580217294303e+18</v>
+        <v>9.663035790814536e+17</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>1eDeCouverture</t>
+          <t>TAMOS_AI_38</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>288</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Paris</t>
-        </is>
-      </c>
+        <v>2214</v>
+      </c>
+      <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Like an anti #Trump on his "madness", one of my subscribers replies: "Who repatriates soldiers, who does not submit ... https://t.co/CZkkpIoFZl </t>
+          <t xml:space="preserve">@ EdRaposo1 There is absolutely nothing confirmed. Contrary to what the media reports there. WHO DECIDES IS MI… https://t.co/e148rLNWg2 </t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t xml:space="preserve">A la ❓d'un anti #Trump sur sa "folie", l'une de mes abonnées répond : "Qui rapatrie les soldats, qui ne se soumet p… </t>
+          <t xml:space="preserve"> Não existe absolutamente nada confirmado. Ao contrário do que a mídia veicula por aí. QUEM DECIDE É O MI… </t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Like an anti #Trump on his "madness", one of my subscribers replies: "Who repatriates soldiers, who does not submit ...  </t>
+          <t xml:space="preserve"> EdRaposo1 There is absolutely nothing confirmed. Contrary to what the media reports there. WHO DECIDES IS MI…  </t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">@ EdRaposo1 There is absolutely nothing confirmed. Contrary to what the media reports there. WHO DECIDES IS MI…  </t>
         </is>
       </c>
     </row>
@@ -626,18 +625,18 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>RT @news_ntd: White House press secretary responds to whether #Trump will acknowledge #Biden as #president-elect
-https://t.co/qPfBgigBJz</t>
+          <t>RT @VoicePoliticsmg: A bust water pipe could delay Georgia vote count, no ballots ruined.
+#USAElections2020 #Biden #Trump #PresidentialEle…</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.33911628746145e+18</v>
+        <v>1.339123245291885e+18</v>
       </c>
       <c r="D4" t="n">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>44181.3284375</v>
+        <v>44181.34763888889</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -645,35 +644,35 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>28803556</v>
+        <v>217271936</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Syunrou</t>
+          <t>MelissaAtwoodTx</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>618</v>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Nagaoka-City, Niigata, Japan</t>
-        </is>
-      </c>
+        <v>310</v>
+      </c>
+      <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @news_ntd: White House press secretary responds to whether #Trump will acknowledge #Biden as #president-electhttps://t.co/qPfBgigBJz </t>
+          <t xml:space="preserve">RT @VoicePoliticsmg: A burst water pipe could delay Georgia vote count, no ballots ruined.#USAElections2020 #Biden #Trump #PresidentialEle… </t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> White House press secretary responds to whether #Trump will acknowledge #Biden as #president-elect
-</t>
+          <t xml:space="preserve"> A bust water pipe could delay Georgia vote count, no ballots ruined.  #USAElections2020 #Biden #Trump #PresidentialEle…</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> White House press secretary responds to whether #Trump will acknowledge #Biden as #president-elect </t>
+          <t xml:space="preserve"> A burst water pipe could delay Georgia vote count, no ballots ruined.#USAElections2020 #Biden #Trump #PresidentialEle… </t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RT @VoicePoliticsmg: A burst water pipe could delay Georgia vote count, no ballots ruined.#USAElections2020 #Biden #Trump #PresidentialEle… </t>
         </is>
       </c>
     </row>
@@ -683,50 +682,53 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>I may just a tiny dust to President Trump as a foriener,
-My donation is unacceptable to #Trump, but my heart for Tr… https://t.co/ndIpvevYtJ</t>
+          <t>RT @DLFNachrichten: In der Causa #Woelki fordert der Münsteraner Kirchenrechtler Schueller Konsequenzen. Woelki leide offenbar an Realitäts…</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1.339116281253917e+18</v>
+        <v>1.339123205227811e+18</v>
       </c>
       <c r="D5" t="n">
         <v>140</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>44181.32841435185</v>
+        <v>44181.34752314815</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>de</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>1.321640627977613e+18</v>
+        <v>3769471457</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>AdeleTWin</t>
+          <t>smartie1944</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>113</v>
+        <v>44</v>
       </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr">
         <is>
-          <t xml:space="preserve">I may just a tiny dust to President Trump as a foreigner,My donation is unacceptable to #Trump, but my heart for Tr… https://t.co/ndIpvevYtJ </t>
+          <t xml:space="preserve">RT @DLFNachrichten: In the case of #Woelki, the Muenster canon lawyer Schueller demands consequences. Woelki apparently suffers from reality ... </t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t xml:space="preserve">I may just a tiny dust to President Trump as a foriener,
-My donation is unacceptable to #Trump, but my heart for Tr… </t>
+          <t xml:space="preserve"> In der Causa #Woelki fordert der Münsteraner Kirchenrechtler Schueller Konsequenzen. Woelki leide offenbar an Realitäts…</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t xml:space="preserve">I may just a tiny dust to President Trump as a foreigner,My donation is unacceptable to #Trump, but my heart for Tr…  </t>
+          <t xml:space="preserve"> In the case of #Woelki, the Muenster canon lawyer Schueller demands consequences. Woelki apparently suffers from reality ... </t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RT @DLFNachrichten: In the case of #Woelki, the Muenster canon lawyer Schueller demands consequences. Woelki apparently suffers from reality ... </t>
         </is>
       </c>
     </row>
@@ -736,48 +738,345 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>RT @gDesFaits: Biden en Géorgie aujourd’hui ! Et on veut nous faire croire que ça va être le nouveau président et qu’il a obtenu 80 million…</t>
+          <t>RT @Trump_Fact_News: Melania #Trump va à l'hôpital pour lire des histoires a des enfants malades, aucun média ne couvre l'événement à part…</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1.33911626612095e+18</v>
+        <v>1.33912319722097e+18</v>
       </c>
       <c r="D6" t="n">
+        <v>139</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>44181.3475</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>fr</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>376695755</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>WhyAlwaysMeHaha</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>182</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RT @Trump_Fact_News: Melania #Trump goes to the hospital to read stories to sick children, no media is covering the event except ... </t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Melania #Trump va à l'hôpital pour lire des histoires a des enfants malades, aucun média ne couvre l'événement à part…</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Melania #Trump goes to the hospital to read stories to sick children, no media is covering the event except ... </t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RT @Trump_Fact_News: Melania #Trump goes to the hospital to read stories to sick children, no media is covering the event except ... </t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>📢 Včera se pravděpodobně #Brexit posunul na #Deal stranu. Graf mluví jasně. Do toho se rýsuje #US #Stimulus (po fin… https://t.co/USIcrbI8uO</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1.339123162261414e+18</v>
+      </c>
+      <c r="D7" t="n">
         <v>140</v>
       </c>
-      <c r="E6" s="2" t="n">
-        <v>44181.32837962963</v>
-      </c>
-      <c r="F6" t="inlineStr">
+      <c r="E7" s="2" t="n">
+        <v>44181.3474074074</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>cs</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>212985092</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>alan_kooper</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>429</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Czech Republic</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">📢 Yesterday, #Brexit probably moved to the #Deal side. The graph speaks clearly. #US #Stimulus is outlined (after fin… https://t.co/USIcrbI8uO </t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">📢 Včera se pravděpodobně #Brexit posunul na #Deal stranu. Graf mluví jasně. Do toho se rýsuje #US #Stimulus (po fin… </t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">📢 Yesterday, #Brexit probably moved to the #Deal side. The graph speaks clearly. #US #Stimulus is outlined (after fin…  </t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">📢 Yesterday, #Brexit probably moved to the #Deal side. The graph speaks clearly. #US #Stimulus is outlined (after fin…  </t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>RT @Trump_Fact_News: Donc on voudrait nous faire croire que ce vieil homme sénile que les médias appellent "Président des Etats-unis" a fai…</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1.339123160621478e+18</v>
+      </c>
+      <c r="D8" t="n">
+        <v>140</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>44181.34739583333</v>
+      </c>
+      <c r="F8" t="inlineStr">
         <is>
           <t>fr</t>
         </is>
       </c>
-      <c r="G6" t="n">
-        <v>310473863</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>frombergers</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>626</v>
-      </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">RT @gDesFaits: Biden in Georgia today! And they want us to believe that this is going to be the new president and that he got 80 million ... </t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Biden en Géorgie aujourd’hui ! Et on veut nous faire croire que ça va être le nouveau président et qu’il a obtenu 80 million…</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Biden in Georgia today! And they want us to believe that this is going to be the new president and that he got 80 million ... </t>
+      <c r="G8" t="n">
+        <v>1.294368775165424e+18</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>NoUseFo90037094</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>81</v>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RT @Trump_Fact_News: So we would like to make us believe that this senile old man whom the media calls "President of the United States" did… </t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Donc on voudrait nous faire croire que ce vieil homme sénile que les médias appellent "Président des Etats-unis" a fai…</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> So we would like to make us believe that this senile old man whom the media calls "President of the United States" did… </t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RT @Trump_Fact_News: So we would like to make us believe that this senile old man whom the media calls "President of the United States" did… </t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Microsoft Fixes Xbox Series X 4K Blu-Ray Brightness Bug SEE MORE HERE ==&amp;gt; https://t.co/uTKq3jCQuw #nintendoswitch… https://t.co/LcCuPRHQhP</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1.339123147484881e+18</v>
+      </c>
+      <c r="D9" t="n">
+        <v>141</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>44181.34736111111</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>306127388</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>bitcoinconnect</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>1253</v>
+      </c>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Microsoft Fixes Xbox Series X 4K Blu-Ray Brightness Bug SEE MORE HERE ==&amp;gt; https://t.co/uTKq3jCQuw #nintendoswitch… https://t.co/LcCuPRHQhP </t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Microsoft Fixes Xbox Series X 4K Blu-Ray Brightness Bug SEE MORE HERE ==&amp;gt;  #nintendoswitch… </t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Microsoft Fixes Xbox Series X 4K Blu-Ray Brightness Bug SEE MORE HERE ==&amp;gt;  #nintendoswitch…  </t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Microsoft Fixes Xbox Series X 4K Blu-Ray Brightness Bug SEE MORE HERE ==&amp;gt;  #nintendoswitch…  </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>RT @bitcoinconnect: I thought the PS5 DualSense controller was a gimmick — until I played this game SEE MORE HERE ==&amp;gt; https://t.co/8PTOFMzQ…</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1.339123096993853e+18</v>
+      </c>
+      <c r="D10" t="n">
+        <v>143</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>44181.34722222222</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>1.332740896199238e+18</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>XboxRetweeter</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>396</v>
+      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RT @bitcoinconnect: I thought the PS5 DualSense controller was a gimmick — until I played this game SEE MORE HERE ==&amp;gt; https://t.co/8PTOFMzQ… </t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> I thought the PS5 DualSense controller was a gimmick — until I played this game SEE MORE HERE ==&amp;gt; …</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> I thought the PS5 DualSense controller was a gimmick — until I played this game SEE MORE HERE ==&amp;gt; … </t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RT @bitcoinconnect: I thought the PS5 DualSense controller was a gimmick — until I played this game SEE MORE HERE ==&amp;gt; … </t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Don't be part of the surrender caucus, fight for #America, @senatemajldr. #Trump was cheated, reclaim republican vi… https://t.co/JAJjxBhIFE</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1.339123056816443e+18</v>
+      </c>
+      <c r="D11" t="n">
+        <v>140</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>44181.34711805556</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>35138538</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>marcvincens</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>116</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Don't be part of the surrender caucus, fight for #America, @senatemajldr. #Trump was cheated, reclaim republican vi… https://t.co/JAJjxBhIFE </t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Don't be part of the surrender caucus, fight for #America, . #Trump was cheated, reclaim republican vi… </t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Don't be part of the surrender caucus, fight for #America, . #Trump was cheated, reclaim republican vi…  </t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Don't be part of the surrender caucus, fight for #America, @senatemajldr. #Trump was cheated, reclaim republican vi…  </t>
         </is>
       </c>
     </row>

</xml_diff>